<commit_message>
change shift register to pcf
</commit_message>
<xml_diff>
--- a/pinout.xlsx
+++ b/pinout.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hubic\Documents\projet_domotique_pauline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hubic\Documents\projet_domotique_pauline\dom_ard_home_automation_wired\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA1C584-7480-4003-B7E7-4E467D55A679}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9757C7C-5274-4B93-A2CB-05002E7AC348}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="230">
   <si>
     <t>Pin Number</t>
   </si>
@@ -708,6 +708,15 @@
   </si>
   <si>
     <t>I2C relay</t>
+  </si>
+  <si>
+    <t>repos</t>
+  </si>
+  <si>
+    <t>actif</t>
+  </si>
+  <si>
+    <t>nombre</t>
   </si>
 </sst>
 </file>
@@ -984,6 +993,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -995,14 +1012,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1353,7 +1362,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1370,14 +1379,25 @@
         <v>218</v>
       </c>
     </row>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D2" t="s">
+        <v>229</v>
+      </c>
+    </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7"/>
@@ -1391,13 +1411,13 @@
       <c r="E4" s="7"/>
     </row>
     <row r="6" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="28" t="s">
         <v>183</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30"/>
     </row>
     <row r="7" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -1432,13 +1452,13 @@
       <c r="E8" s="7"/>
     </row>
     <row r="10" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="31" t="s">
         <v>187</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -1544,13 +1564,13 @@
       <c r="E17" s="7"/>
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="31" t="s">
         <v>194</v>
       </c>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
@@ -1591,7 +1611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="X34:X39"/>
   <sheetViews>
-    <sheetView topLeftCell="D21" zoomScale="65" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="65" workbookViewId="0">
       <selection activeCell="Z36" sqref="Z36"/>
     </sheetView>
   </sheetViews>
@@ -1630,8 +1650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1FEC41E-48DC-4C4E-8511-81BECF32536B}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="E78" sqref="E74:E78"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D90" sqref="D42:D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2962,26 +2982,26 @@
       <c r="E97" s="7"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="28">
+      <c r="A98" s="24">
         <v>97</v>
       </c>
-      <c r="B98" s="28" t="s">
+      <c r="B98" s="24" t="s">
         <v>162</v>
       </c>
       <c r="C98" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="D98" s="29"/>
-      <c r="E98" s="30"/>
+      <c r="D98" s="25"/>
+      <c r="E98" s="26"/>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A99" s="31">
+      <c r="A99" s="27">
         <v>98</v>
       </c>
-      <c r="B99" s="31" t="s">
+      <c r="B99" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="C99" s="31" t="s">
+      <c r="C99" s="27" t="s">
         <v>165</v>
       </c>
       <c r="D99" s="7"/>

</xml_diff>